<commit_message>
Add content examples from old templates
No checklist creation possible due to bug https://github.com/nfdi4plants/Swate/issues/180 .
</commit_message>
<xml_diff>
--- a/templates/3ASY01_RNASeq/3ASY01_RNASeq.xlsx
+++ b/templates/3ASY01_RNASeq/3ASY01_RNASeq.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\omaus\SWATE_templates\templates\3ASY01_RNASeq\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2368526-59A1-40B9-BCDC-8D44C04B8FB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4556D474-90B2-4BE2-B8F6-8DBCD33E8959}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="171">
   <si>
     <t>Source Name</t>
   </si>
@@ -305,9 +305,6 @@
   </si>
   <si>
     <t>Dominik</t>
-  </si>
-  <si>
-    <t>1.1.4</t>
   </si>
   <si>
     <t/>
@@ -592,6 +589,81 @@
   <si>
     <t>RAW FILES_file name</t>
   </si>
+  <si>
+    <t>RNA-Seq strategy</t>
+  </si>
+  <si>
+    <t>ChIP-Seq strategy</t>
+  </si>
+  <si>
+    <t>ssRNA-seq</t>
+  </si>
+  <si>
+    <t>cDNA method</t>
+  </si>
+  <si>
+    <t>size fractionation method</t>
+  </si>
+  <si>
+    <t>PolyA</t>
+  </si>
+  <si>
+    <t>rRNA depletion</t>
+  </si>
+  <si>
+    <t>Paired-end</t>
+  </si>
+  <si>
+    <t>Single-end</t>
+  </si>
+  <si>
+    <t>Illumina TrueSeq</t>
+  </si>
+  <si>
+    <t>ACTTGA</t>
+  </si>
+  <si>
+    <t>TAGCTT</t>
+  </si>
+  <si>
+    <t>CGTACG</t>
+  </si>
+  <si>
+    <t>HiSeq 2000</t>
+  </si>
+  <si>
+    <t>Illumina Casava</t>
+  </si>
+  <si>
+    <t>1.70</t>
+  </si>
+  <si>
+    <t>R1</t>
+  </si>
+  <si>
+    <t>R2</t>
+  </si>
+  <si>
+    <t>Forward</t>
+  </si>
+  <si>
+    <t>Parameter [Base-calling Software version]</t>
+  </si>
+  <si>
+    <t>Term Source REF (NFDI4PSO:0000018)</t>
+  </si>
+  <si>
+    <t>Term Accession Number (NFDI4PSO:0000018)</t>
+  </si>
+  <si>
+    <t>.fastq</t>
+  </si>
+  <si>
+    <t>.ab1</t>
+  </si>
+  <si>
+    <t>1.1.5</t>
+  </si>
 </sst>
 </file>
 
@@ -600,7 +672,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.00\ &quot;microgram&quot;"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -612,6 +684,19 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFF5F5F5"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -743,10 +828,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -785,11 +871,13 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Normal 3" xfId="1" xr:uid="{3A68927A-4D0F-438E-A11A-69BC80D82D4C}"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="23">
+  <dxfs count="26">
     <dxf>
       <numFmt numFmtId="164" formatCode="0.00\ &quot;microgram&quot;"/>
     </dxf>
@@ -818,7 +906,16 @@
       <numFmt numFmtId="164" formatCode="0.00\ &quot;microgram&quot;"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="164" formatCode="0.00\ &quot;microgram&quot;"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.00\ &quot;microgram&quot;"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="0.00\ &quot;microgram&quot;"/>
@@ -879,9 +976,9 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{FF8CF88B-39F4-4BB8-A79A-D46E92AF4094}" name="annotationTableSpicySloth85" displayName="annotationTableSpicySloth85" ref="A1:AP2" totalsRowShown="0">
-  <autoFilter ref="A1:AP2" xr:uid="{FF8CF88B-39F4-4BB8-A79A-D46E92AF4094}"/>
-  <tableColumns count="42">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{FF8CF88B-39F4-4BB8-A79A-D46E92AF4094}" name="annotationTableSpicySloth85" displayName="annotationTableSpicySloth85" ref="A1:AS5" totalsRowShown="0">
+  <autoFilter ref="A1:AS5" xr:uid="{FF8CF88B-39F4-4BB8-A79A-D46E92AF4094}"/>
+  <tableColumns count="45">
     <tableColumn id="1" xr3:uid="{DDD81922-E978-4A5A-A247-30D8EC830850}" name="Source Name"/>
     <tableColumn id="3" xr3:uid="{447A413B-B655-4E5D-BC02-D7557A9E4C62}" name="Parameter [Library strategy]"/>
     <tableColumn id="4" xr3:uid="{9BBFE835-D0D7-4C6D-A1A5-68598432EDA2}" name="Term Source REF (NFDI4PSO:0000035)"/>
@@ -901,19 +998,22 @@
     <tableColumn id="18" xr3:uid="{89B6BCBB-C5AD-4373-B0EA-160F3BBCA468}" name="Parameter [Adapter sequence]"/>
     <tableColumn id="19" xr3:uid="{7C720ACC-EDDD-4B8C-B7F4-F21BDC9B0FFF}" name="Term Source REF (NFDI4PSO:0000039)"/>
     <tableColumn id="20" xr3:uid="{743BF0E4-CDEB-4353-988F-B91A1D110B43}" name="Term Accession Number (NFDI4PSO:0000039)"/>
-    <tableColumn id="21" xr3:uid="{C2221C5A-A581-47B0-99E1-8D8101F1F64D}" name="Parameter [Library RNA amount]" dataDxfId="22"/>
-    <tableColumn id="22" xr3:uid="{406988CC-530E-4763-91F9-71C83D968873}" name="Unit" dataDxfId="21"/>
-    <tableColumn id="23" xr3:uid="{05065244-1A82-4F1F-B9B7-0A69AAE33604}" name="Term Source REF (NFDI4PSO:0000016)" dataDxfId="20"/>
-    <tableColumn id="24" xr3:uid="{6CD94A2D-03CE-49DA-96F8-3F68DB81454E}" name="Term Accession Number (NFDI4PSO:0000016)" dataDxfId="19"/>
-    <tableColumn id="25" xr3:uid="{541AA4B9-BAFF-430B-8B9A-F2C021B53404}" name="Parameter [rRNA depletion]" dataDxfId="18"/>
-    <tableColumn id="26" xr3:uid="{2CE133DA-0A67-40F6-A2D3-5E44ECC584FE}" name="Term Source REF (NFDI4PSO:0000082)" dataDxfId="17"/>
-    <tableColumn id="27" xr3:uid="{7E102C7E-3D48-4AE3-B973-C93CF504F0EE}" name="Term Accession Number (NFDI4PSO:0000082)" dataDxfId="16"/>
-    <tableColumn id="28" xr3:uid="{9C794364-C911-4D05-A9A8-DFDE330A09C2}" name="Parameter [Next generation sequencing instrument model]" dataDxfId="15"/>
-    <tableColumn id="29" xr3:uid="{AE615784-B0E6-47BF-AE01-023BF5AA206E}" name="Term Source REF (NFDI4PSO:0000040)" dataDxfId="14"/>
-    <tableColumn id="30" xr3:uid="{BAD8DB17-65F5-45BD-A7AA-6B024B5CE069}" name="Term Accession Number (NFDI4PSO:0000040)" dataDxfId="13"/>
-    <tableColumn id="31" xr3:uid="{9791FFA0-96AA-41FF-837C-5CD04C7414C8}" name="Parameter [Base-calling Software]" dataDxfId="12"/>
-    <tableColumn id="32" xr3:uid="{482633AE-33E1-4455-8BC3-9D5A09A98094}" name="Term Source REF (NFDI4PSO:0000017)" dataDxfId="11"/>
-    <tableColumn id="33" xr3:uid="{98CB4042-CD1B-4E0C-B718-7E81226BF0F8}" name="Term Accession Number (NFDI4PSO:0000017)" dataDxfId="10"/>
+    <tableColumn id="21" xr3:uid="{C2221C5A-A581-47B0-99E1-8D8101F1F64D}" name="Parameter [Library RNA amount]" dataDxfId="25"/>
+    <tableColumn id="22" xr3:uid="{406988CC-530E-4763-91F9-71C83D968873}" name="Unit" dataDxfId="24"/>
+    <tableColumn id="23" xr3:uid="{05065244-1A82-4F1F-B9B7-0A69AAE33604}" name="Term Source REF (NFDI4PSO:0000016)" dataDxfId="23"/>
+    <tableColumn id="24" xr3:uid="{6CD94A2D-03CE-49DA-96F8-3F68DB81454E}" name="Term Accession Number (NFDI4PSO:0000016)" dataDxfId="22"/>
+    <tableColumn id="25" xr3:uid="{541AA4B9-BAFF-430B-8B9A-F2C021B53404}" name="Parameter [rRNA depletion]" dataDxfId="21"/>
+    <tableColumn id="26" xr3:uid="{2CE133DA-0A67-40F6-A2D3-5E44ECC584FE}" name="Term Source REF (NFDI4PSO:0000082)" dataDxfId="20"/>
+    <tableColumn id="27" xr3:uid="{7E102C7E-3D48-4AE3-B973-C93CF504F0EE}" name="Term Accession Number (NFDI4PSO:0000082)" dataDxfId="19"/>
+    <tableColumn id="28" xr3:uid="{9C794364-C911-4D05-A9A8-DFDE330A09C2}" name="Parameter [Next generation sequencing instrument model]" dataDxfId="18"/>
+    <tableColumn id="29" xr3:uid="{AE615784-B0E6-47BF-AE01-023BF5AA206E}" name="Term Source REF (NFDI4PSO:0000040)" dataDxfId="17"/>
+    <tableColumn id="30" xr3:uid="{BAD8DB17-65F5-45BD-A7AA-6B024B5CE069}" name="Term Accession Number (NFDI4PSO:0000040)" dataDxfId="16"/>
+    <tableColumn id="31" xr3:uid="{9791FFA0-96AA-41FF-837C-5CD04C7414C8}" name="Parameter [Base-calling Software]" dataDxfId="15"/>
+    <tableColumn id="32" xr3:uid="{482633AE-33E1-4455-8BC3-9D5A09A98094}" name="Term Source REF (NFDI4PSO:0000017)" dataDxfId="14"/>
+    <tableColumn id="33" xr3:uid="{98CB4042-CD1B-4E0C-B718-7E81226BF0F8}" name="Term Accession Number (NFDI4PSO:0000017)" dataDxfId="13"/>
+    <tableColumn id="50" xr3:uid="{3CCB5926-3B22-468E-A9A9-17F469915A9F}" name="Parameter [Base-calling Software version]" dataDxfId="12"/>
+    <tableColumn id="51" xr3:uid="{9873F5F5-4534-4DF9-B18C-69858B28E021}" name="Term Source REF (NFDI4PSO:0000018)" dataDxfId="11"/>
+    <tableColumn id="52" xr3:uid="{E50595D3-C218-4183-8EC4-0B001A8697BD}" name="Term Accession Number (NFDI4PSO:0000018)" dataDxfId="10"/>
     <tableColumn id="34" xr3:uid="{228D9D5B-B4BB-432B-8766-144F2F7EE00C}" name="Parameter [Base-calling Software Parameters]" dataDxfId="9"/>
     <tableColumn id="35" xr3:uid="{EE5985B1-BFA8-4880-80F1-BBC5E373AEA4}" name="Term Source REF (NFDI4PSO:0000019)" dataDxfId="8"/>
     <tableColumn id="36" xr3:uid="{5957DE4F-4101-47BD-A1D2-8A8C3805387F}" name="Term Accession Number (NFDI4PSO:0000019)" dataDxfId="7"/>
@@ -1203,8 +1303,11 @@
 
 <file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
 <wetp:taskpanes xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
-  <wetp:taskpane dockstate="right" visibility="0" width="350" row="0">
+  <wetp:taskpane dockstate="right" visibility="0" width="625" row="2">
     <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+  </wetp:taskpane>
+  <wetp:taskpane dockstate="right" visibility="0" width="643" row="3">
+    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
   </wetp:taskpane>
 </wetp:taskpanes>
 </file>
@@ -1219,9 +1322,19 @@
 </we:webextension>
 </file>
 
+<file path=xl/webextensions/webextension2.xml><?xml version="1.0" encoding="utf-8"?>
+<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{E6E17174-D1EE-42AD-8695-B7125DABAE59}">
+  <we:reference id="5d6f5462-3401-48ec-9406-d12882e9ad84" version="0.5.1.0" store="\\DT-P-2020-04-OM\swate_manifests" storeType="Filesystem"/>
+  <we:alternateReferences/>
+  <we:properties/>
+  <we:bindings/>
+  <we:snapshot xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
+</we:webextension>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AP2"/>
+  <dimension ref="A1:AS5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1259,19 +1372,21 @@
     <col min="30" max="30" width="34" bestFit="1" customWidth="1"/>
     <col min="31" max="31" width="36.7109375" hidden="1" customWidth="1"/>
     <col min="32" max="32" width="43.7109375" hidden="1" customWidth="1"/>
-    <col min="33" max="33" width="44.85546875" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="36.7109375" hidden="1" customWidth="1"/>
-    <col min="35" max="35" width="43.7109375" hidden="1" customWidth="1"/>
-    <col min="36" max="36" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="43.7109375" style="14" customWidth="1"/>
+    <col min="34" max="35" width="43.7109375" hidden="1" customWidth="1"/>
+    <col min="36" max="36" width="44.85546875" style="14" bestFit="1" customWidth="1"/>
     <col min="37" max="37" width="36.7109375" hidden="1" customWidth="1"/>
     <col min="38" max="38" width="43.7109375" hidden="1" customWidth="1"/>
-    <col min="39" max="39" width="32.7109375" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="26.7109375" bestFit="1" customWidth="1"/>
     <col min="40" max="40" width="36.7109375" hidden="1" customWidth="1"/>
     <col min="41" max="41" width="43.7109375" hidden="1" customWidth="1"/>
-    <col min="42" max="42" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="32.7109375" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="36.7109375" hidden="1" customWidth="1"/>
+    <col min="44" max="44" width="43.7109375" hidden="1" customWidth="1"/>
+    <col min="45" max="45" width="16.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1368,38 +1483,62 @@
       <c r="AF1" t="s">
         <v>31</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AG1" s="14" t="s">
+        <v>165</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>166</v>
+      </c>
+      <c r="AI1" t="s">
+        <v>167</v>
+      </c>
+      <c r="AJ1" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AK1" t="s">
         <v>33</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AL1" t="s">
         <v>34</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="AM1" t="s">
         <v>35</v>
       </c>
-      <c r="AK1" t="s">
+      <c r="AN1" t="s">
         <v>36</v>
       </c>
-      <c r="AL1" t="s">
+      <c r="AO1" t="s">
         <v>37</v>
       </c>
-      <c r="AM1" t="s">
+      <c r="AP1" t="s">
         <v>38</v>
       </c>
-      <c r="AN1" t="s">
+      <c r="AQ1" t="s">
         <v>39</v>
       </c>
-      <c r="AO1" t="s">
+      <c r="AR1" t="s">
         <v>40</v>
       </c>
-      <c r="AP1" t="s">
+      <c r="AS1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>146</v>
+      </c>
+      <c r="E2" t="s">
+        <v>149</v>
+      </c>
+      <c r="H2" t="s">
+        <v>153</v>
+      </c>
+      <c r="K2" t="s">
+        <v>155</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>156</v>
+      </c>
       <c r="T2" s="1"/>
       <c r="U2" s="1"/>
       <c r="V2" s="1"/>
@@ -1407,24 +1546,145 @@
       <c r="X2" s="1"/>
       <c r="Y2" s="1"/>
       <c r="Z2" s="1"/>
-      <c r="AA2" s="1"/>
+      <c r="AA2" s="1" t="s">
+        <v>159</v>
+      </c>
       <c r="AB2" s="1"/>
       <c r="AC2" s="1"/>
-      <c r="AD2" s="1"/>
+      <c r="AD2" s="1" t="s">
+        <v>160</v>
+      </c>
       <c r="AE2" s="1"/>
       <c r="AF2" s="1"/>
-      <c r="AG2" s="1"/>
+      <c r="AG2" s="14" t="s">
+        <v>161</v>
+      </c>
       <c r="AH2" s="1"/>
       <c r="AI2" s="1"/>
-      <c r="AJ2" s="1"/>
       <c r="AK2" s="1"/>
       <c r="AL2" s="1"/>
-      <c r="AM2" s="1"/>
+      <c r="AM2" s="1" t="s">
+        <v>162</v>
+      </c>
       <c r="AN2" s="1"/>
       <c r="AO2" s="1"/>
-      <c r="AP2" s="1"/>
+      <c r="AP2" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="AQ2" s="1"/>
+      <c r="AR2" s="1"/>
+      <c r="AS2" s="1"/>
+    </row>
+    <row r="3" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>147</v>
+      </c>
+      <c r="E3" t="s">
+        <v>150</v>
+      </c>
+      <c r="H3" t="s">
+        <v>154</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>157</v>
+      </c>
+      <c r="T3" s="1"/>
+      <c r="U3" s="1"/>
+      <c r="V3" s="1"/>
+      <c r="W3" s="1"/>
+      <c r="X3" s="1"/>
+      <c r="Y3" s="1"/>
+      <c r="Z3" s="1"/>
+      <c r="AA3" s="1"/>
+      <c r="AB3" s="1"/>
+      <c r="AC3" s="1"/>
+      <c r="AD3" s="1"/>
+      <c r="AE3" s="1"/>
+      <c r="AF3" s="1"/>
+      <c r="AH3" s="1"/>
+      <c r="AI3" s="1"/>
+      <c r="AK3" s="1"/>
+      <c r="AL3" s="1"/>
+      <c r="AM3" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="AN3" s="1"/>
+      <c r="AO3" s="1"/>
+      <c r="AP3" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="AQ3" s="1"/>
+      <c r="AR3" s="1"/>
+      <c r="AS3" s="1"/>
+    </row>
+    <row r="4" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>148</v>
+      </c>
+      <c r="E4" t="s">
+        <v>151</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>158</v>
+      </c>
+      <c r="T4" s="1"/>
+      <c r="U4" s="1"/>
+      <c r="V4" s="1"/>
+      <c r="W4" s="1"/>
+      <c r="X4" s="1"/>
+      <c r="Y4" s="1"/>
+      <c r="Z4" s="1"/>
+      <c r="AA4" s="1"/>
+      <c r="AB4" s="1"/>
+      <c r="AC4" s="1"/>
+      <c r="AD4" s="1"/>
+      <c r="AE4" s="1"/>
+      <c r="AF4" s="1"/>
+      <c r="AH4" s="1"/>
+      <c r="AI4" s="1"/>
+      <c r="AK4" s="1"/>
+      <c r="AL4" s="1"/>
+      <c r="AM4" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="AN4" s="1"/>
+      <c r="AO4" s="1"/>
+      <c r="AP4" s="1"/>
+      <c r="AQ4" s="1"/>
+      <c r="AR4" s="1"/>
+      <c r="AS4" s="1"/>
+    </row>
+    <row r="5" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="E5" t="s">
+        <v>152</v>
+      </c>
+      <c r="T5" s="1"/>
+      <c r="U5" s="1"/>
+      <c r="V5" s="1"/>
+      <c r="W5" s="1"/>
+      <c r="X5" s="1"/>
+      <c r="Y5" s="1"/>
+      <c r="Z5" s="1"/>
+      <c r="AA5" s="1"/>
+      <c r="AB5" s="1"/>
+      <c r="AC5" s="1"/>
+      <c r="AD5" s="1"/>
+      <c r="AE5" s="1"/>
+      <c r="AF5" s="1"/>
+      <c r="AH5" s="1"/>
+      <c r="AI5" s="1"/>
+      <c r="AK5" s="1"/>
+      <c r="AL5" s="1"/>
+      <c r="AM5" s="1"/>
+      <c r="AN5" s="1"/>
+      <c r="AO5" s="1"/>
+      <c r="AP5" s="1"/>
+      <c r="AQ5" s="1"/>
+      <c r="AR5" s="1"/>
+      <c r="AS5" s="1"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
@@ -1465,7 +1725,7 @@
         <v>44</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>83</v>
+        <v>170</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -1690,40 +1950,40 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="B1" s="12" t="s">
         <v>84</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="C1" s="12" t="s">
         <v>85</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="D1" s="12" t="s">
         <v>86</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="E1" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="F1" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="F1" s="12" t="s">
+      <c r="G1" s="12" t="s">
         <v>89</v>
       </c>
-      <c r="G1" s="12" t="s">
+      <c r="H1" s="12" t="s">
         <v>90</v>
       </c>
-      <c r="H1" s="12" t="s">
+      <c r="I1" s="12" t="s">
         <v>91</v>
       </c>
-      <c r="I1" s="12" t="s">
+      <c r="J1" s="12" t="s">
         <v>92</v>
       </c>
-      <c r="J1" s="12" t="s">
+      <c r="K1" s="12" t="s">
         <v>93</v>
       </c>
-      <c r="K1" s="12" t="s">
+      <c r="L1" s="12" t="s">
         <v>94</v>
-      </c>
-      <c r="L1" s="12" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
@@ -1731,13 +1991,13 @@
         <v>0</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C2" s="13" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D2" s="13" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E2" s="13"/>
       <c r="F2" s="13"/>
@@ -1750,16 +2010,16 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D3" s="13" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E3" s="13"/>
       <c r="F3" s="13"/>
@@ -1775,29 +2035,29 @@
         <v>1</v>
       </c>
       <c r="B4" s="13" t="s">
+        <v>96</v>
+      </c>
+      <c r="C4" s="13" t="s">
         <v>97</v>
       </c>
-      <c r="C4" s="13" t="s">
+      <c r="D4" s="13" t="s">
         <v>98</v>
       </c>
-      <c r="D4" s="13" t="s">
-        <v>99</v>
-      </c>
       <c r="E4" s="13" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F4" s="13"/>
       <c r="G4" s="13" t="s">
+        <v>127</v>
+      </c>
+      <c r="H4" s="13" t="s">
         <v>128</v>
       </c>
-      <c r="H4" s="13" t="s">
+      <c r="I4" s="13" t="s">
         <v>129</v>
       </c>
-      <c r="I4" s="13" t="s">
+      <c r="J4" s="13" t="s">
         <v>130</v>
-      </c>
-      <c r="J4" s="13" t="s">
-        <v>131</v>
       </c>
       <c r="K4" s="13"/>
       <c r="L4" s="13"/>
@@ -1807,29 +2067,29 @@
         <v>4</v>
       </c>
       <c r="B5" s="13" t="s">
+        <v>99</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="D5" s="13" t="s">
         <v>100</v>
       </c>
-      <c r="C5" s="13" t="s">
-        <v>98</v>
-      </c>
-      <c r="D5" s="13" t="s">
-        <v>101</v>
-      </c>
       <c r="E5" s="13" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F5" s="13"/>
       <c r="G5" s="13" t="s">
+        <v>131</v>
+      </c>
+      <c r="H5" s="13" t="s">
         <v>132</v>
       </c>
-      <c r="H5" s="13" t="s">
+      <c r="I5" s="13" t="s">
+        <v>129</v>
+      </c>
+      <c r="J5" s="13" t="s">
         <v>133</v>
-      </c>
-      <c r="I5" s="13" t="s">
-        <v>130</v>
-      </c>
-      <c r="J5" s="13" t="s">
-        <v>134</v>
       </c>
       <c r="K5" s="13"/>
       <c r="L5" s="13"/>
@@ -1839,29 +2099,29 @@
         <v>7</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D6" s="13" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E6" s="13"/>
       <c r="F6" s="13" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="G6" s="13" t="s">
+        <v>134</v>
+      </c>
+      <c r="H6" s="13" t="s">
         <v>135</v>
       </c>
-      <c r="H6" s="13" t="s">
-        <v>136</v>
-      </c>
       <c r="I6" s="13" t="s">
+        <v>129</v>
+      </c>
+      <c r="J6" s="13" t="s">
         <v>130</v>
-      </c>
-      <c r="J6" s="13" t="s">
-        <v>131</v>
       </c>
       <c r="K6" s="13"/>
       <c r="L6" s="13"/>
@@ -1871,31 +2131,31 @@
         <v>10</v>
       </c>
       <c r="B7" s="13" t="s">
+        <v>102</v>
+      </c>
+      <c r="C7" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="D7" s="13" t="s">
         <v>103</v>
-      </c>
-      <c r="C7" s="13" t="s">
-        <v>98</v>
-      </c>
-      <c r="D7" s="13" t="s">
-        <v>104</v>
       </c>
       <c r="E7" s="13"/>
       <c r="F7" s="13"/>
       <c r="G7" s="13" t="s">
+        <v>131</v>
+      </c>
+      <c r="H7" s="13" t="s">
         <v>132</v>
       </c>
-      <c r="H7" s="13" t="s">
+      <c r="I7" s="13" t="s">
+        <v>129</v>
+      </c>
+      <c r="J7" s="13" t="s">
         <v>133</v>
-      </c>
-      <c r="I7" s="13" t="s">
-        <v>130</v>
-      </c>
-      <c r="J7" s="13" t="s">
-        <v>134</v>
       </c>
       <c r="K7" s="13"/>
       <c r="L7" s="13" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
@@ -1903,27 +2163,27 @@
         <v>13</v>
       </c>
       <c r="B8" s="13" t="s">
+        <v>104</v>
+      </c>
+      <c r="C8" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="D8" s="13" t="s">
         <v>105</v>
-      </c>
-      <c r="C8" s="13" t="s">
-        <v>98</v>
-      </c>
-      <c r="D8" s="13" t="s">
-        <v>106</v>
       </c>
       <c r="E8" s="13"/>
       <c r="F8" s="13"/>
       <c r="G8" s="13" t="s">
+        <v>131</v>
+      </c>
+      <c r="H8" s="13" t="s">
         <v>132</v>
       </c>
-      <c r="H8" s="13" t="s">
+      <c r="I8" s="13" t="s">
+        <v>129</v>
+      </c>
+      <c r="J8" s="13" t="s">
         <v>133</v>
-      </c>
-      <c r="I8" s="13" t="s">
-        <v>130</v>
-      </c>
-      <c r="J8" s="13" t="s">
-        <v>134</v>
       </c>
       <c r="K8" s="13"/>
       <c r="L8" s="13"/>
@@ -1933,27 +2193,27 @@
         <v>16</v>
       </c>
       <c r="B9" s="13" t="s">
+        <v>106</v>
+      </c>
+      <c r="C9" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="D9" s="13" t="s">
         <v>107</v>
-      </c>
-      <c r="C9" s="13" t="s">
-        <v>98</v>
-      </c>
-      <c r="D9" s="13" t="s">
-        <v>108</v>
       </c>
       <c r="E9" s="13"/>
       <c r="F9" s="13"/>
       <c r="G9" s="13" t="s">
+        <v>131</v>
+      </c>
+      <c r="H9" s="13" t="s">
         <v>132</v>
       </c>
-      <c r="H9" s="13" t="s">
+      <c r="I9" s="13" t="s">
+        <v>129</v>
+      </c>
+      <c r="J9" s="13" t="s">
         <v>133</v>
-      </c>
-      <c r="I9" s="13" t="s">
-        <v>130</v>
-      </c>
-      <c r="J9" s="13" t="s">
-        <v>134</v>
       </c>
       <c r="K9" s="13"/>
       <c r="L9" s="13"/>
@@ -1963,29 +2223,29 @@
         <v>19</v>
       </c>
       <c r="B10" s="13" t="s">
+        <v>108</v>
+      </c>
+      <c r="C10" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="D10" s="13" t="s">
         <v>109</v>
       </c>
-      <c r="C10" s="13" t="s">
-        <v>98</v>
-      </c>
-      <c r="D10" s="13" t="s">
-        <v>110</v>
-      </c>
       <c r="E10" s="13" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F10" s="13"/>
       <c r="G10" s="13" t="s">
+        <v>131</v>
+      </c>
+      <c r="H10" s="13" t="s">
         <v>132</v>
       </c>
-      <c r="H10" s="13" t="s">
+      <c r="I10" s="13" t="s">
+        <v>129</v>
+      </c>
+      <c r="J10" s="13" t="s">
         <v>133</v>
-      </c>
-      <c r="I10" s="13" t="s">
-        <v>130</v>
-      </c>
-      <c r="J10" s="13" t="s">
-        <v>134</v>
       </c>
       <c r="K10" s="13"/>
       <c r="L10" s="13"/>
@@ -1995,27 +2255,27 @@
         <v>23</v>
       </c>
       <c r="B11" s="13" t="s">
+        <v>110</v>
+      </c>
+      <c r="C11" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="D11" s="13" t="s">
         <v>111</v>
-      </c>
-      <c r="C11" s="13" t="s">
-        <v>98</v>
-      </c>
-      <c r="D11" s="13" t="s">
-        <v>112</v>
       </c>
       <c r="E11" s="13"/>
       <c r="F11" s="13"/>
       <c r="G11" s="13" t="s">
+        <v>131</v>
+      </c>
+      <c r="H11" s="13" t="s">
         <v>132</v>
       </c>
-      <c r="H11" s="13" t="s">
+      <c r="I11" s="13" t="s">
+        <v>129</v>
+      </c>
+      <c r="J11" s="13" t="s">
         <v>133</v>
-      </c>
-      <c r="I11" s="13" t="s">
-        <v>130</v>
-      </c>
-      <c r="J11" s="13" t="s">
-        <v>134</v>
       </c>
       <c r="K11" s="13"/>
       <c r="L11" s="13"/>
@@ -2025,27 +2285,27 @@
         <v>26</v>
       </c>
       <c r="B12" s="13" t="s">
+        <v>112</v>
+      </c>
+      <c r="C12" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="D12" s="13" t="s">
         <v>113</v>
-      </c>
-      <c r="C12" s="13" t="s">
-        <v>98</v>
-      </c>
-      <c r="D12" s="13" t="s">
-        <v>114</v>
       </c>
       <c r="E12" s="13"/>
       <c r="F12" s="13"/>
       <c r="G12" s="13" t="s">
+        <v>137</v>
+      </c>
+      <c r="H12" s="13" t="s">
         <v>138</v>
       </c>
-      <c r="H12" s="13" t="s">
-        <v>139</v>
-      </c>
       <c r="I12" s="13" t="s">
+        <v>129</v>
+      </c>
+      <c r="J12" s="13" t="s">
         <v>130</v>
-      </c>
-      <c r="J12" s="13" t="s">
-        <v>131</v>
       </c>
       <c r="K12" s="13"/>
       <c r="L12" s="13"/>
@@ -2055,64 +2315,64 @@
         <v>29</v>
       </c>
       <c r="B13" s="13" t="s">
+        <v>114</v>
+      </c>
+      <c r="C13" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="D13" s="13" t="s">
         <v>115</v>
       </c>
-      <c r="C13" s="13" t="s">
-        <v>98</v>
-      </c>
-      <c r="D13" s="13" t="s">
-        <v>116</v>
-      </c>
       <c r="E13" s="13" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F13" s="13"/>
       <c r="G13" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="H13" s="13" t="s">
         <v>140</v>
       </c>
-      <c r="H13" s="13" t="s">
+      <c r="I13" s="13" t="s">
         <v>141</v>
       </c>
-      <c r="I13" s="13" t="s">
+      <c r="J13" s="13" t="s">
+        <v>133</v>
+      </c>
+      <c r="K13" s="13" t="s">
         <v>142</v>
-      </c>
-      <c r="J13" s="13" t="s">
-        <v>134</v>
-      </c>
-      <c r="K13" s="13" t="s">
-        <v>143</v>
       </c>
       <c r="L13" s="13"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="12" t="s">
+        <v>116</v>
+      </c>
+      <c r="B14" s="13" t="s">
         <v>117</v>
       </c>
-      <c r="B14" s="13" t="s">
+      <c r="C14" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="D14" s="13" t="s">
         <v>118</v>
-      </c>
-      <c r="C14" s="13" t="s">
-        <v>98</v>
-      </c>
-      <c r="D14" s="13" t="s">
-        <v>119</v>
       </c>
       <c r="E14" s="13"/>
       <c r="F14" s="13"/>
       <c r="G14" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="H14" s="13" t="s">
         <v>140</v>
       </c>
-      <c r="H14" s="13" t="s">
+      <c r="I14" s="13" t="s">
         <v>141</v>
       </c>
-      <c r="I14" s="13" t="s">
+      <c r="J14" s="13" t="s">
+        <v>133</v>
+      </c>
+      <c r="K14" s="13" t="s">
         <v>142</v>
-      </c>
-      <c r="J14" s="13" t="s">
-        <v>134</v>
-      </c>
-      <c r="K14" s="13" t="s">
-        <v>143</v>
       </c>
       <c r="L14" s="13"/>
     </row>
@@ -2121,30 +2381,30 @@
         <v>32</v>
       </c>
       <c r="B15" s="13" t="s">
+        <v>119</v>
+      </c>
+      <c r="C15" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="D15" s="13" t="s">
         <v>120</v>
-      </c>
-      <c r="C15" s="13" t="s">
-        <v>98</v>
-      </c>
-      <c r="D15" s="13" t="s">
-        <v>121</v>
       </c>
       <c r="E15" s="13"/>
       <c r="F15" s="13"/>
       <c r="G15" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="H15" s="13" t="s">
         <v>140</v>
       </c>
-      <c r="H15" s="13" t="s">
+      <c r="I15" s="13" t="s">
         <v>141</v>
       </c>
-      <c r="I15" s="13" t="s">
+      <c r="J15" s="13" t="s">
+        <v>133</v>
+      </c>
+      <c r="K15" s="13" t="s">
         <v>142</v>
-      </c>
-      <c r="J15" s="13" t="s">
-        <v>134</v>
-      </c>
-      <c r="K15" s="13" t="s">
-        <v>143</v>
       </c>
       <c r="L15" s="13"/>
     </row>
@@ -2153,27 +2413,27 @@
         <v>35</v>
       </c>
       <c r="B16" s="13" t="s">
+        <v>121</v>
+      </c>
+      <c r="C16" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="D16" s="13" t="s">
         <v>122</v>
-      </c>
-      <c r="C16" s="13" t="s">
-        <v>98</v>
-      </c>
-      <c r="D16" s="13" t="s">
-        <v>123</v>
       </c>
       <c r="E16" s="13"/>
       <c r="F16" s="13"/>
       <c r="G16" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="H16" s="13" t="s">
         <v>140</v>
       </c>
-      <c r="H16" s="13" t="s">
+      <c r="I16" s="13" t="s">
         <v>141</v>
       </c>
-      <c r="I16" s="13" t="s">
-        <v>142</v>
-      </c>
       <c r="J16" s="13" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="K16" s="13"/>
       <c r="L16" s="13"/>
@@ -2183,27 +2443,27 @@
         <v>38</v>
       </c>
       <c r="B17" s="13" t="s">
+        <v>123</v>
+      </c>
+      <c r="C17" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="D17" s="13" t="s">
         <v>124</v>
-      </c>
-      <c r="C17" s="13" t="s">
-        <v>98</v>
-      </c>
-      <c r="D17" s="13" t="s">
-        <v>125</v>
       </c>
       <c r="E17" s="13"/>
       <c r="F17" s="13"/>
       <c r="G17" s="13" t="s">
+        <v>143</v>
+      </c>
+      <c r="H17" s="13" t="s">
         <v>144</v>
       </c>
-      <c r="H17" s="13" t="s">
-        <v>145</v>
-      </c>
       <c r="I17" s="13" t="s">
+        <v>129</v>
+      </c>
+      <c r="J17" s="13" t="s">
         <v>130</v>
-      </c>
-      <c r="J17" s="13" t="s">
-        <v>131</v>
       </c>
       <c r="K17" s="13"/>
       <c r="L17" s="13"/>
@@ -2213,25 +2473,25 @@
         <v>41</v>
       </c>
       <c r="B18" s="13" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C18" s="13" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D18" s="13" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E18" s="13"/>
       <c r="F18" s="13"/>
       <c r="G18" s="13" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="H18" s="13"/>
       <c r="I18" s="13" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="J18" s="13" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="K18" s="13"/>
       <c r="L18" s="13"/>

</xml_diff>